<commit_message>
update bug , commit erd
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -33,9 +33,6 @@
     <t>Button invite in Invite popup</t>
   </si>
   <si>
-    <t>New</t>
-  </si>
-  <si>
     <t>Detail</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Cannot accept any answer</t>
+  </si>
+  <si>
+    <t>Resolved</t>
   </si>
 </sst>
 </file>
@@ -134,6 +134,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -182,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,7 +220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -429,7 +432,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +455,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -463,16 +466,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -480,16 +483,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -497,16 +500,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -514,16 +517,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -531,16 +534,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -548,16 +551,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -565,16 +568,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -582,16 +585,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,16 +602,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>